<commit_message>
fix: SE3-SE3A direction swapped
</commit_message>
<xml_diff>
--- a/data/map_ig107-intradayNTC.xlsx
+++ b/data/map_ig107-intradayNTC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nordicrsc-my.sharepoint.com/personal/jlm_nordic-rcc_net/Documents/Dokumenter/topology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="8_{D11A41F1-3D3A-40FE-8D66-E136A7A41780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3832F27-4E19-41B6-BD25-5FE42437AEDE}"/>
+  <xr:revisionPtr revIDLastSave="200" documentId="8_{D11A41F1-3D3A-40FE-8D66-E136A7A41780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E083DD9A-5FF8-4930-B6D3-045E85345D4E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{879DBF62-5915-4E1B-BB81-2834436B8A2E}"/>
+    <workbookView xWindow="28680" yWindow="-5490" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{879DBF62-5915-4E1B-BB81-2834436B8A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="metaData" sheetId="1" r:id="rId1"/>
@@ -354,7 +354,7 @@
     <t>mapCreatedDate</t>
   </si>
   <si>
-    <t>2024-08-12</t>
+    <t>2024-10-02</t>
   </si>
 </sst>
 </file>
@@ -807,16 +807,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A7284C-B5FB-484E-A2B3-0244298D3E3F}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="10" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -848,7 +848,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -856,7 +856,7 @@
         <v>104</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D2" t="s">
         <v>75</v>
@@ -880,13 +880,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C9" s="1"/>
     </row>
   </sheetData>
@@ -901,18 +901,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D153D6-6422-49A5-92A2-7897A0750DDC}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -920,7 +920,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
@@ -928,7 +928,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>80</v>
       </c>
@@ -936,7 +936,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>85</v>
       </c>
@@ -945,7 +945,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>79</v>
       </c>
@@ -954,7 +954,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -963,7 +963,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>78</v>
       </c>
@@ -972,7 +972,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>50</v>
       </c>
@@ -980,7 +980,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>51</v>
       </c>
@@ -988,7 +988,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>81</v>
       </c>
@@ -997,7 +997,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>82</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>83</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>92</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>76</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>84</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>87</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>52</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>86</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>9</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>11</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>12</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>13</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>14</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>15</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>16</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>17</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>20</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>93</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>21</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>22</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>23</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>24</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>25</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>26</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>27</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>31</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>32</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>88</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>28</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>89</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>30</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>70</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>34</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>35</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>33</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>94</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>95</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>73</v>
       </c>
@@ -1391,23 +1391,23 @@
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B61" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>96</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>97</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>100</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>101</v>
       </c>

</xml_diff>